<commit_message>
aggiunto Hygenic Clamp Tee
</commit_message>
<xml_diff>
--- a/data/Tees and reducers.xlsx
+++ b/data/Tees and reducers.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5b494536d0e93f0f/Documenti/DKW Pharma/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="8_{3D5B90C2-5B50-45D4-9A98-A1A193031E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5E09919-12C3-41BC-B183-CE0378BBF186}"/>
+  <xr:revisionPtr revIDLastSave="142" documentId="8_{3D5B90C2-5B50-45D4-9A98-A1A193031E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86F332F0-0708-486A-AB74-7115193D65EF}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16860" activeTab="2" xr2:uid="{FCC25AD9-9076-4FCD-A086-0E3A82E1FE1A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16860" activeTab="3" xr2:uid="{FCC25AD9-9076-4FCD-A086-0E3A82E1FE1A}"/>
   </bookViews>
   <sheets>
     <sheet name="Tees" sheetId="1" r:id="rId1"/>
     <sheet name="Conc. Reducers" sheetId="2" r:id="rId2"/>
     <sheet name="Ecc. Reducers" sheetId="3" r:id="rId3"/>
+    <sheet name="Outlet Hyg. Clamp - Red. Tees " sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="340">
   <si>
     <t xml:space="preserve"> ASME BPE SF1 (BF) Code</t>
   </si>
@@ -831,12 +832,386 @@
   <si>
     <t>SF4-RE-96-64-3-1</t>
   </si>
+  <si>
+    <r>
+      <t>DT-4.1.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Grandview"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">2-7 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color indexed="23"/>
+        <rFont val="Grandview"/>
+        <family val="2"/>
+      </rPr>
+      <t>Short Outlet Hygienic Clamp, Joint Reducing Tee</t>
+    </r>
+  </si>
+  <si>
+    <t>Nominal Sizes</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Grandview"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFE30613"/>
+        <rFont val="Webdings"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Grandview"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> ASME BPE SF1 (BF)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Grandview"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFE30613"/>
+        <rFont val="Webdings"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Grandview"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> ASME BPE SF4 (EP)</t>
+    </r>
+  </si>
+  <si>
+    <t>SF1-TR-06-04-2-7</t>
+  </si>
+  <si>
+    <t>on request</t>
+  </si>
+  <si>
+    <t>SF4-TR-06-04-2-7</t>
+  </si>
+  <si>
+    <t>SF1-TR-08-04-2-7</t>
+  </si>
+  <si>
+    <t>SF4-TR-08-04-2-7</t>
+  </si>
+  <si>
+    <t>SF1-TR-08-06-2-7</t>
+  </si>
+  <si>
+    <t>SF4-TR-08-06-2-7</t>
+  </si>
+  <si>
+    <t>SF1-TR-12-04-2-7</t>
+  </si>
+  <si>
+    <t>SF4-TR-12-04-2-7</t>
+  </si>
+  <si>
+    <t>SF1-TR-12-06-2-7</t>
+  </si>
+  <si>
+    <t>SF4-TR-12-06-2-7</t>
+  </si>
+  <si>
+    <t>SF1-TR-12-08-2-7</t>
+  </si>
+  <si>
+    <t>SF4-TR-12-08-2-7</t>
+  </si>
+  <si>
+    <t>SF1-TR-16-08-2-7</t>
+  </si>
+  <si>
+    <t>SF4-TR-16-08-2-7</t>
+  </si>
+  <si>
+    <t>SF1-TR-16-12-2-7</t>
+  </si>
+  <si>
+    <t>SF4-TR-16-12-2-7</t>
+  </si>
+  <si>
+    <t>SF1-TR-24-08-2-7</t>
+  </si>
+  <si>
+    <t>SF4-TR-24-08-2-7</t>
+  </si>
+  <si>
+    <t>SF1-TR-24-12-2-7</t>
+  </si>
+  <si>
+    <t>SF4-TR-24-12-2-7</t>
+  </si>
+  <si>
+    <t>SF1-TR-24-16-2-7</t>
+  </si>
+  <si>
+    <t>SF4-TR-24-16-2-7</t>
+  </si>
+  <si>
+    <t>SF1-TR-32-08-2-7</t>
+  </si>
+  <si>
+    <t>SF4-TR-32-08-2-7</t>
+  </si>
+  <si>
+    <t>SF1-TR-32-12-2-7</t>
+  </si>
+  <si>
+    <t>SF4-TR-32-12-2-7</t>
+  </si>
+  <si>
+    <t>SF1-TR-32-16-2-7</t>
+  </si>
+  <si>
+    <t>SF4-TR-32-16-2-7</t>
+  </si>
+  <si>
+    <t>SF1-TR-32-24-2-7</t>
+  </si>
+  <si>
+    <t>SF4-TR-32-24-2-7</t>
+  </si>
+  <si>
+    <t>SF1-TR-40-08-2-7</t>
+  </si>
+  <si>
+    <t>SF4-TR-40-08-2-7</t>
+  </si>
+  <si>
+    <t>SF1-TR-40-12-2-7</t>
+  </si>
+  <si>
+    <t>SF4-TR-40-12-2-7</t>
+  </si>
+  <si>
+    <t>SF1-TR-40-16-2-7</t>
+  </si>
+  <si>
+    <t>SF4-TR-40-16-2-7</t>
+  </si>
+  <si>
+    <t>SF1-TR-40-24-2-7</t>
+  </si>
+  <si>
+    <t>SF4-TR-40-24-2-7</t>
+  </si>
+  <si>
+    <t>SF1-TR-40-32-2-7</t>
+  </si>
+  <si>
+    <t>SF4-TR-40-32-2-7</t>
+  </si>
+  <si>
+    <t>SF1-TR-48-08-2-7</t>
+  </si>
+  <si>
+    <t>SF4-TR-48-08-2-7</t>
+  </si>
+  <si>
+    <t>SF1-TR-48-12-2-7</t>
+  </si>
+  <si>
+    <t>SF4-TR-48-12-2-7</t>
+  </si>
+  <si>
+    <t>SF1-TR-48-16-2-7</t>
+  </si>
+  <si>
+    <t>SF4-TR-48-16-2-7</t>
+  </si>
+  <si>
+    <t>SF1-TR-48-24-2-7</t>
+  </si>
+  <si>
+    <t>SF4-TR-48-24-2-7</t>
+  </si>
+  <si>
+    <t>SF1-TR-48-32-2-7</t>
+  </si>
+  <si>
+    <t>SF4-TR-48-32-2-7</t>
+  </si>
+  <si>
+    <t>SF1-TR-48-40-2-7</t>
+  </si>
+  <si>
+    <t>SF4-TR-48-40-2-7</t>
+  </si>
+  <si>
+    <t>SF1-TR-64-08-2-7</t>
+  </si>
+  <si>
+    <t>SF4-TR-64-08-2-7</t>
+  </si>
+  <si>
+    <t>SF1-TR-64-12-2-7</t>
+  </si>
+  <si>
+    <t>SF4-TR-64-12-2-7</t>
+  </si>
+  <si>
+    <t>SF1-TR-64-16-2-7</t>
+  </si>
+  <si>
+    <t>SF4-TR-64-16-2-7</t>
+  </si>
+  <si>
+    <t>SF1-TR-64-24-2-7</t>
+  </si>
+  <si>
+    <t>SF4-TR-64-24-2-7</t>
+  </si>
+  <si>
+    <t>SF1-TR-64-32-2-7</t>
+  </si>
+  <si>
+    <t>SF4-TR-64-32-2-7</t>
+  </si>
+  <si>
+    <t>SF1-TR-64-40-2-7</t>
+  </si>
+  <si>
+    <t>SF4-TR-64-40-2-7</t>
+  </si>
+  <si>
+    <t>SF1-TR-64-48-2-7</t>
+  </si>
+  <si>
+    <t>SF4-TR-64-48-2-7</t>
+  </si>
+  <si>
+    <t>SF1-TR-96-12-2-7</t>
+  </si>
+  <si>
+    <t>SF4-TR-96-12-2-7</t>
+  </si>
+  <si>
+    <t>SF1-TR-96-16-2-7</t>
+  </si>
+  <si>
+    <t>SF4-TR-96-16-2-7</t>
+  </si>
+  <si>
+    <t>SF1-TR-96-24-2-7</t>
+  </si>
+  <si>
+    <t>SF4-TR-96-24-2-7</t>
+  </si>
+  <si>
+    <t>SF1-TR-96-32-2-7</t>
+  </si>
+  <si>
+    <t>SF4-TR-96-32-2-7</t>
+  </si>
+  <si>
+    <t>SF1-TR-96-40-2-7</t>
+  </si>
+  <si>
+    <t>SF4-TR-96-40-2-7</t>
+  </si>
+  <si>
+    <t>SF1-TR-96-48-2-7</t>
+  </si>
+  <si>
+    <t>SF4-TR-96-48-2-7</t>
+  </si>
+  <si>
+    <t>SF1-TR-96-64-2-7</t>
+  </si>
+  <si>
+    <t>SF4-TR-96-64-2-7</t>
+  </si>
+  <si>
+    <t>6.35</t>
+  </si>
+  <si>
+    <t>12.70</t>
+  </si>
+  <si>
+    <t>9.53</t>
+  </si>
+  <si>
+    <t>19.05</t>
+  </si>
+  <si>
+    <t>25.40</t>
+  </si>
+  <si>
+    <t>38.10</t>
+  </si>
+  <si>
+    <t>50.80</t>
+  </si>
+  <si>
+    <t>11/2"</t>
+  </si>
+  <si>
+    <t>63.50</t>
+  </si>
+  <si>
+    <t>76.20</t>
+  </si>
+  <si>
+    <t>101.60</t>
+  </si>
+  <si>
+    <t>152.40</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -904,6 +1279,26 @@
       <name val="Grandview"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <name val="Grandview"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Grandview"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFE30613"/>
+      <name val="Webdings"/>
+      <family val="1"/>
+      <charset val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -925,7 +1320,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -1083,12 +1478,94 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1131,8 +1608,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1148,6 +1625,50 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1207,6 +1728,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1529,7 +2054,7 @@
   <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I1048576"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3604,7 +4129,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89514210-54F1-4589-8AC3-AC6DFF9CD907}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
@@ -4208,13 +4733,8 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:H23">
     <sortCondition ref="B3:B23"/>
   </sortState>
-  <conditionalFormatting sqref="A3:D23">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3:H23">
-    <cfRule type="expression" dxfId="0" priority="1">
+  <conditionalFormatting sqref="A3:H23">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4223,4 +4743,1198 @@
     <ignoredError sqref="B3:D23" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47AF5B8E-ED68-4EF1-9FA0-0B4733F63F2F}">
+  <dimension ref="A1:N43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="4" width="13.453125" customWidth="1"/>
+    <col min="5" max="5" width="8.6328125" customWidth="1"/>
+    <col min="6" max="6" width="22.54296875" customWidth="1"/>
+    <col min="7" max="7" width="25.7265625" customWidth="1"/>
+    <col min="8" max="8" width="22.54296875" customWidth="1"/>
+    <col min="9" max="9" width="29.54296875" customWidth="1"/>
+    <col min="11" max="14" width="16.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="25" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="28"/>
+      <c r="K1" t="e">
+        <f>MID(A1, 1, SEARCH(" x", A1)-1)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L1" t="e">
+        <f>TRIM(RIGHT(A1,LEN(A1)-FIND("x",A1)))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M1" t="e">
+        <f>MID(B1, 1, SEARCH(" x", B1)-1)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N1" t="e">
+        <f>TRIM(RIGHT(B1,LEN(B1)-FIND("x",B1)))</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" s="29" t="s">
+        <v>244</v>
+      </c>
+      <c r="B2" s="30"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="32" t="s">
+        <v>245</v>
+      </c>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33" t="s">
+        <v>246</v>
+      </c>
+      <c r="I2" s="34"/>
+    </row>
+    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A4" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>328</v>
+      </c>
+      <c r="E4" s="36"/>
+      <c r="F4" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A5" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="43" t="s">
+        <v>328</v>
+      </c>
+      <c r="E5" s="37"/>
+      <c r="F5" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A6" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="43" t="s">
+        <v>330</v>
+      </c>
+      <c r="E6" s="37"/>
+      <c r="F6" s="16" t="s">
+        <v>252</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>253</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A7" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="43" t="s">
+        <v>328</v>
+      </c>
+      <c r="E7" s="37"/>
+      <c r="F7" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>255</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A8" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="43" t="s">
+        <v>330</v>
+      </c>
+      <c r="E8" s="37"/>
+      <c r="F8" s="16" t="s">
+        <v>256</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>257</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A9" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="C9" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="43" t="s">
+        <v>329</v>
+      </c>
+      <c r="E9" s="37"/>
+      <c r="F9" s="16" t="s">
+        <v>258</v>
+      </c>
+      <c r="G9" s="14">
+        <v>60.314995253157782</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>259</v>
+      </c>
+      <c r="I9" s="15">
+        <v>82.739034238714595</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A10" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="C10" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="43" t="s">
+        <v>329</v>
+      </c>
+      <c r="E10" s="37"/>
+      <c r="F10" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="G10" s="14">
+        <v>45.786554497646577</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>261</v>
+      </c>
+      <c r="I10" s="15">
+        <v>69.857145286438239</v>
+      </c>
+      <c r="M10" s="44"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A11" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="43" t="s">
+        <v>331</v>
+      </c>
+      <c r="E11" s="37"/>
+      <c r="F11" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="G11" s="14">
+        <v>45.016636457020411</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="I11" s="15">
+        <v>69.053820248645692</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A12" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>333</v>
+      </c>
+      <c r="C12" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="42" t="s">
+        <v>329</v>
+      </c>
+      <c r="E12" s="36"/>
+      <c r="F12" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="G12" s="10">
+        <v>56.691107971005103</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="I12" s="11">
+        <v>84.381261969727134</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A13" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>333</v>
+      </c>
+      <c r="C13" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="42" t="s">
+        <v>331</v>
+      </c>
+      <c r="E13" s="36"/>
+      <c r="F13" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="G13" s="10">
+        <v>48.897651886299293</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="I13" s="11">
+        <v>76.267679088022604</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A14" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>333</v>
+      </c>
+      <c r="C14" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="42" t="s">
+        <v>332</v>
+      </c>
+      <c r="E14" s="36"/>
+      <c r="F14" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="G14" s="10">
+        <v>44.74952203476235</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="I14" s="11">
+        <v>71.94579038469881</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A15" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="C15" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="42" t="s">
+        <v>329</v>
+      </c>
+      <c r="E15" s="36"/>
+      <c r="F15" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="G15" s="10">
+        <v>53.957113296128483</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="I15" s="11">
+        <v>86.277109058917503</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A16" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="C16" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="43" t="s">
+        <v>331</v>
+      </c>
+      <c r="E16" s="37"/>
+      <c r="F16" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="G16" s="14">
+        <v>53.957113296128483</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="I16" s="15">
+        <v>86.277109058917503</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="C17" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="43" t="s">
+        <v>332</v>
+      </c>
+      <c r="E17" s="37"/>
+      <c r="F17" s="16" t="s">
+        <v>274</v>
+      </c>
+      <c r="G17" s="14">
+        <v>52.794379928652219</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>275</v>
+      </c>
+      <c r="I17" s="15">
+        <v>85.072121502228711</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="C18" s="39" t="s">
+        <v>335</v>
+      </c>
+      <c r="D18" s="43" t="s">
+        <v>333</v>
+      </c>
+      <c r="E18" s="37"/>
+      <c r="F18" s="16" t="s">
+        <v>276</v>
+      </c>
+      <c r="G18" s="14">
+        <v>52.794379928652219</v>
+      </c>
+      <c r="H18" s="16" t="s">
+        <v>277</v>
+      </c>
+      <c r="I18" s="15">
+        <v>85.072121502228711</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="C19" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="43" t="s">
+        <v>329</v>
+      </c>
+      <c r="E19" s="37"/>
+      <c r="F19" s="16" t="s">
+        <v>278</v>
+      </c>
+      <c r="G19" s="14">
+        <v>66.935731695255484</v>
+      </c>
+      <c r="H19" s="16" t="s">
+        <v>279</v>
+      </c>
+      <c r="I19" s="15">
+        <v>107.70982106722217</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="C20" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="43" t="s">
+        <v>331</v>
+      </c>
+      <c r="E20" s="37"/>
+      <c r="F20" s="16" t="s">
+        <v>280</v>
+      </c>
+      <c r="G20" s="14">
+        <v>66.935731695255484</v>
+      </c>
+      <c r="H20" s="16" t="s">
+        <v>281</v>
+      </c>
+      <c r="I20" s="15">
+        <v>107.70982106722217</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="C21" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="43" t="s">
+        <v>332</v>
+      </c>
+      <c r="E21" s="37"/>
+      <c r="F21" s="16" t="s">
+        <v>282</v>
+      </c>
+      <c r="G21" s="14">
+        <v>66.668617272997409</v>
+      </c>
+      <c r="H21" s="16" t="s">
+        <v>283</v>
+      </c>
+      <c r="I21" s="15">
+        <v>107.4366905543727</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="C22" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="43" t="s">
+        <v>333</v>
+      </c>
+      <c r="E22" s="37"/>
+      <c r="F22" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="G22" s="14">
+        <v>67.45424792669759</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>285</v>
+      </c>
+      <c r="I22" s="15">
+        <v>108.24001559216526</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="C23" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="42" t="s">
+        <v>334</v>
+      </c>
+      <c r="E23" s="36"/>
+      <c r="F23" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="G23" s="10">
+        <v>73.802143608595074</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="I23" s="11">
+        <v>114.87548040433151</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>337</v>
+      </c>
+      <c r="C24" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="42" t="s">
+        <v>329</v>
+      </c>
+      <c r="E24" s="36"/>
+      <c r="F24" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="G24" s="10">
+        <v>80.558567230416628</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="I24" s="11">
+        <v>126.65222545836997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>337</v>
+      </c>
+      <c r="C25" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="42" t="s">
+        <v>331</v>
+      </c>
+      <c r="E25" s="36"/>
+      <c r="F25" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="G25" s="10">
+        <v>80.558567230416628</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="I25" s="11">
+        <v>126.65222545836997</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>337</v>
+      </c>
+      <c r="C26" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="42" t="s">
+        <v>332</v>
+      </c>
+      <c r="E26" s="36"/>
+      <c r="F26" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="G26" s="10">
+        <v>81.721300597892906</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="I26" s="11">
+        <v>127.85721301505876</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="C27" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="43" t="s">
+        <v>333</v>
+      </c>
+      <c r="E27" s="37"/>
+      <c r="F27" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="G27" s="14">
+        <v>81.721300597892906</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="I27" s="15">
+        <v>127.85721301505876</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="C28" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="43" t="s">
+        <v>334</v>
+      </c>
+      <c r="E28" s="37"/>
+      <c r="F28" s="16" t="s">
+        <v>296</v>
+      </c>
+      <c r="G28" s="14">
+        <v>88.210609797456371</v>
+      </c>
+      <c r="H28" s="16" t="s">
+        <v>297</v>
+      </c>
+      <c r="I28" s="15">
+        <v>134.62120983327188</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="C29" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="43" t="s">
+        <v>336</v>
+      </c>
+      <c r="E29" s="37"/>
+      <c r="F29" s="16" t="s">
+        <v>298</v>
+      </c>
+      <c r="G29" s="14">
+        <v>92.610141458177409</v>
+      </c>
+      <c r="H29" s="16" t="s">
+        <v>299</v>
+      </c>
+      <c r="I29" s="15">
+        <v>139.23229555020097</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="C30" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="43" t="s">
+        <v>329</v>
+      </c>
+      <c r="E30" s="37"/>
+      <c r="F30" s="16" t="s">
+        <v>300</v>
+      </c>
+      <c r="G30" s="14">
+        <v>142.41912490276891</v>
+      </c>
+      <c r="H30" s="16" t="s">
+        <v>301</v>
+      </c>
+      <c r="I30" s="15">
+        <v>197.47336079015921</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="C31" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="43" t="s">
+        <v>331</v>
+      </c>
+      <c r="E31" s="37"/>
+      <c r="F31" s="16" t="s">
+        <v>302</v>
+      </c>
+      <c r="G31" s="14">
+        <v>142.41912490276891</v>
+      </c>
+      <c r="H31" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="I31" s="15">
+        <v>197.47336079015921</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="C32" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="43" t="s">
+        <v>332</v>
+      </c>
+      <c r="E32" s="37"/>
+      <c r="F32" s="16" t="s">
+        <v>304</v>
+      </c>
+      <c r="G32" s="14">
+        <v>117.26323137128909</v>
+      </c>
+      <c r="H32" s="16" t="s">
+        <v>305</v>
+      </c>
+      <c r="I32" s="15">
+        <v>171.23676505585527</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A33" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="C33" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="43" t="s">
+        <v>333</v>
+      </c>
+      <c r="E33" s="37"/>
+      <c r="F33" s="13" t="s">
+        <v>306</v>
+      </c>
+      <c r="G33" s="14">
+        <v>117.26323137128909</v>
+      </c>
+      <c r="H33" s="13" t="s">
+        <v>307</v>
+      </c>
+      <c r="I33" s="15">
+        <v>171.23676505585527</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A34" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="C34" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="42" t="s">
+        <v>334</v>
+      </c>
+      <c r="E34" s="36"/>
+      <c r="F34" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="G34" s="10">
+        <v>123.61112705318659</v>
+      </c>
+      <c r="H34" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="I34" s="11">
+        <v>177.87222986802155</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A35" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="C35" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="42" t="s">
+        <v>336</v>
+      </c>
+      <c r="E35" s="36"/>
+      <c r="F35" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="G35" s="10">
+        <v>126.59652353724726</v>
+      </c>
+      <c r="H35" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="I35" s="11">
+        <v>180.97306451390074</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A36" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="C36" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" s="42" t="s">
+        <v>337</v>
+      </c>
+      <c r="E36" s="36"/>
+      <c r="F36" s="9" t="s">
+        <v>312</v>
+      </c>
+      <c r="G36" s="10">
+        <v>131.53028404248442</v>
+      </c>
+      <c r="H36" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="I36" s="11">
+        <v>186.11434475577289</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A37" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="C37" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="42" t="s">
+        <v>331</v>
+      </c>
+      <c r="E37" s="36"/>
+      <c r="F37" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="G37" s="10">
+        <v>373.0488596029943</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="I37" s="11">
+        <v>538.75796984593683</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A38" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="C38" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="43" t="s">
+        <v>332</v>
+      </c>
+      <c r="E38" s="37"/>
+      <c r="F38" s="13" t="s">
+        <v>316</v>
+      </c>
+      <c r="G38" s="14">
+        <v>371.1162081948919</v>
+      </c>
+      <c r="H38" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="I38" s="15">
+        <v>536.73359075069959</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A39" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="C39" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="43" t="s">
+        <v>333</v>
+      </c>
+      <c r="E39" s="37"/>
+      <c r="F39" s="16" t="s">
+        <v>318</v>
+      </c>
+      <c r="G39" s="14">
+        <v>371.1159949636338</v>
+      </c>
+      <c r="H39" s="16" t="s">
+        <v>319</v>
+      </c>
+      <c r="I39" s="15">
+        <v>536.73359075069959</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A40" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="C40" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" s="43" t="s">
+        <v>334</v>
+      </c>
+      <c r="E40" s="37"/>
+      <c r="F40" s="16" t="s">
+        <v>320</v>
+      </c>
+      <c r="G40" s="14">
+        <v>377.46410387678924</v>
+      </c>
+      <c r="H40" s="16" t="s">
+        <v>321</v>
+      </c>
+      <c r="I40" s="15">
+        <v>543.35298906211005</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A41" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="C41" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" s="42" t="s">
+        <v>336</v>
+      </c>
+      <c r="E41" s="36"/>
+      <c r="F41" s="9" t="s">
+        <v>322</v>
+      </c>
+      <c r="G41" s="10">
+        <v>380.44950036084987</v>
+      </c>
+      <c r="H41" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="I41" s="11">
+        <v>546.46989020874503</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A42" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="C42" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="D42" s="43" t="s">
+        <v>337</v>
+      </c>
+      <c r="E42" s="37"/>
+      <c r="F42" s="13" t="s">
+        <v>324</v>
+      </c>
+      <c r="G42" s="14">
+        <v>385.50896177067909</v>
+      </c>
+      <c r="H42" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="I42" s="15">
+        <v>551.73970245666419</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A43" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="C43" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43" s="43" t="s">
+        <v>338</v>
+      </c>
+      <c r="E43" s="37"/>
+      <c r="F43" s="16" t="s">
+        <v>326</v>
+      </c>
+      <c r="G43" s="14">
+        <v>385.50896177067909</v>
+      </c>
+      <c r="H43" s="16" t="s">
+        <v>327</v>
+      </c>
+      <c r="I43" s="15">
+        <v>551.73864143403773</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:I43">
+    <sortCondition ref="B4:B43"/>
+  </sortState>
+  <mergeCells count="3">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A4:I43">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="B4:D43" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>